<commit_message>
Updated C# progress file.
</commit_message>
<xml_diff>
--- a/C#_Progress.xlsx
+++ b/C#_Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA0BE4D-2793-4564-8593-3135675C6660}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B210EF-E52A-463F-8E33-A41BBE4DB589}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C91C04C4-F181-44A5-A0F8-4FCE844357C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C91C04C4-F181-44A5-A0F8-4FCE844357C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>New contents</t>
   </si>
@@ -46,10 +46,16 @@
 Convert Console App to Library.</t>
   </si>
   <si>
-    <t>Created "Consignment Shop" App. Research on Collections, Properties, Interfaces and Patterns.</t>
-  </si>
-  <si>
     <t>08/09.12.2019</t>
+  </si>
+  <si>
+    <t>Read into Collections, Linq, Lambda expressions</t>
+  </si>
+  <si>
+    <t>Created "Consignment Shop" App. Research on Properties, Interfaces and Patterns.</t>
+  </si>
+  <si>
+    <t>Review of "Consignment Shop" code, Intial code refactoring, Introduction to basic principles.</t>
   </si>
 </sst>
 </file>
@@ -405,15 +411,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FA41FE-4077-4A52-B21D-318630668283}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -438,15 +445,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43809</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43810</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>